<commit_message>
added openpyxl depenency installation in .yml
</commit_message>
<xml_diff>
--- a/test_data/output/test.xlsx
+++ b/test_data/output/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>reference_position</t>
   </si>
@@ -31,12 +31,6 @@
     <t>allele</t>
   </si>
   <si>
-    <t>linkage</t>
-  </si>
-  <si>
-    <t>zygosity</t>
-  </si>
-  <si>
     <t>allele_count</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>Homozygous</t>
   </si>
   <si>
     <t>45.0</t>
@@ -435,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +434,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,56 +474,46 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s"/>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>